<commit_message>
More stuff and things
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/orders/OrderFiles/US Foods/Formatted _ US Foods _ TRIPHAMMER 01312025.xlsx
+++ b/WorkBot/main/backend/orders/OrderFiles/US Foods/Formatted _ US Foods _ TRIPHAMMER 01312025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,6 +806,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>94154</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>